<commit_message>
Excel project all functions created
</commit_message>
<xml_diff>
--- a/Python classes/excelProject/excelProjectDB.xlsx
+++ b/Python classes/excelProject/excelProjectDB.xlsx
@@ -1,38 +1,100 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="120" yWindow="30" windowWidth="20115" windowHeight="7500" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="120" yWindow="30" windowWidth="20115" windowHeight="7500" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
-    <sheet name="ListOfTrainees" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="CourseDetails" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="TrainerDetails" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="ManagerDetails" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="MappingCourseTrainee" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="MappingCourseTrainer" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="ListOfTrainees" sheetId="1" r:id="rId1"/>
+    <sheet name="CourseDetails" sheetId="2" r:id="rId2"/>
+    <sheet name="TrainerDetails" sheetId="3" r:id="rId3"/>
+    <sheet name="ManagerDetails" sheetId="4" r:id="rId4"/>
+    <sheet name="MappingCourseTrainee" sheetId="5" r:id="rId5"/>
+    <sheet name="MappingCourseTrainer" sheetId="6" r:id="rId6"/>
+    <sheet name="C343 19.03.23" sheetId="7" r:id="rId7"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="144525" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Alex</t>
+  </si>
+  <si>
+    <t>Maths</t>
+  </si>
+  <si>
+    <t>Wiley</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Computing</t>
+  </si>
+  <si>
+    <t>Mthree</t>
+  </si>
+  <si>
+    <t>C343</t>
+  </si>
+  <si>
+    <t>C++ and python</t>
+  </si>
+  <si>
+    <t>hello@gmail.com</t>
+  </si>
+  <si>
+    <t>Alex Smith</t>
+  </si>
+  <si>
+    <t>080092288</t>
+  </si>
+  <si>
+    <t>Hellen@gmail.com</t>
+  </si>
+  <si>
+    <t>Hellen Bell</t>
+  </si>
+  <si>
+    <t>2343</t>
+  </si>
+  <si>
+    <t>19:00</t>
+  </si>
+  <si>
+    <t>22:00</t>
+  </si>
+  <si>
+    <t>Absent</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -51,80 +113,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -414,40 +414,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1"/>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>John</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>maths</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Wiley</t>
-        </is>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -456,91 +455,147 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Excel project bug fixes, session menu works and deletes trainees and trainers properly
</commit_message>
<xml_diff>
--- a/Python classes/excelProject/excelProjectDB.xlsx
+++ b/Python classes/excelProject/excelProjectDB.xlsx
@@ -1,100 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="20115" windowHeight="7500" firstSheet="1" activeTab="6"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="120" yWindow="30" windowWidth="20115" windowHeight="7500" tabRatio="754" firstSheet="1" activeTab="6" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="ListOfTrainees" sheetId="1" r:id="rId1"/>
-    <sheet name="CourseDetails" sheetId="2" r:id="rId2"/>
-    <sheet name="TrainerDetails" sheetId="3" r:id="rId3"/>
-    <sheet name="ManagerDetails" sheetId="4" r:id="rId4"/>
-    <sheet name="MappingCourseTrainee" sheetId="5" r:id="rId5"/>
-    <sheet name="MappingCourseTrainer" sheetId="6" r:id="rId6"/>
-    <sheet name="C343 19.03.23" sheetId="7" r:id="rId7"/>
+    <sheet name="ListOfTrainees" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="CourseDetails" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="TrainerDetails" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="ManagerDetails" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="MappingCourseTrainee" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="MappingCourseTrainer" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="C343 19.03.23" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="C343 22.2.22" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>Alex</t>
-  </si>
-  <si>
-    <t>Maths</t>
-  </si>
-  <si>
-    <t>Wiley</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>John</t>
-  </si>
-  <si>
-    <t>Computing</t>
-  </si>
-  <si>
-    <t>Mthree</t>
-  </si>
-  <si>
-    <t>C343</t>
-  </si>
-  <si>
-    <t>C++ and python</t>
-  </si>
-  <si>
-    <t>hello@gmail.com</t>
-  </si>
-  <si>
-    <t>Alex Smith</t>
-  </si>
-  <si>
-    <t>080092288</t>
-  </si>
-  <si>
-    <t>Hellen@gmail.com</t>
-  </si>
-  <si>
-    <t>Hellen Bell</t>
-  </si>
-  <si>
-    <t>2343</t>
-  </si>
-  <si>
-    <t>19:00</t>
-  </si>
-  <si>
-    <t>22:00</t>
-  </si>
-  <si>
-    <t>Absent</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -113,18 +53,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -414,39 +416,83 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A2:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Alex</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Maths</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Wiley</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>John</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Computing</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Mthree</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Chris</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -455,21 +501,42 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
+    <row r="1"/>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>C343</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>C++ and python</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>C345</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Maths</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -478,22 +545,34 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A2:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>hello@gmail.com</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Alex Smith</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>080092288</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -502,22 +581,34 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A2:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" t="s">
-        <v>15</v>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Hellen@gmail.com</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Hellen Bell</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>2343</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -526,21 +617,41 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>C343</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>C343</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -549,21 +660,29 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A2:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>C343</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>hello@gmail.com</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -572,27 +691,96 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>19:00</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>22:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Absent</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>10:30</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>11:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Absent</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Present</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Excel project manager and email absences
</commit_message>
<xml_diff>
--- a/Python classes/excelProject/excelProjectDB.xlsx
+++ b/Python classes/excelProject/excelProjectDB.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="120" yWindow="30" windowWidth="20115" windowHeight="7500" tabRatio="754" firstSheet="1" activeTab="6" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="120" yWindow="30" windowWidth="20115" windowHeight="7500" tabRatio="754" firstSheet="0" activeTab="6" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="ListOfTrainees" sheetId="1" state="visible" r:id="rId1"/>
@@ -12,8 +12,9 @@
     <sheet name="ManagerDetails" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="MappingCourseTrainee" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="MappingCourseTrainer" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="C343 19.03.23" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="C343 22.2.22" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="MappingCourseManager" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="C343 19.03.23" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="C343 22.2.22" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -586,7 +587,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:C2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -594,20 +595,21 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
+    <row r="1"/>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Hellen@gmail.com</t>
+          <t>Wiley@Wiley.com</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Hellen Bell</t>
+          <t>Wiley Edge</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2343</t>
+          <t>99999</t>
         </is>
       </c>
     </row>
@@ -699,7 +701,39 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="K18" sqref="K18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1"/>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>C343</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Wiley@Wiley.com</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -733,7 +767,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>